<commit_message>
commit for tt jan 14
</commit_message>
<xml_diff>
--- a/curiculam_CE.xlsx
+++ b/curiculam_CE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Python\tempWorkSpace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drlak\my_projects\my_timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAE4CD5-D0E3-48F5-B497-437348E76B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32BC652C-A70C-4703-8141-50CD75147487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12645" yWindow="1695" windowWidth="15435" windowHeight="13590" activeTab="7" xr2:uid="{7BEB5D9E-8563-4ED7-B850-B47E02154E05}"/>
+    <workbookView xWindow="1695" yWindow="3300" windowWidth="22560" windowHeight="10305" activeTab="6" xr2:uid="{7BEB5D9E-8563-4ED7-B850-B47E02154E05}"/>
   </bookViews>
   <sheets>
     <sheet name="s1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="195">
   <si>
     <t>GAMAT101</t>
   </si>
@@ -380,9 +380,6 @@
   </si>
   <si>
     <t>PCITS705</t>
-  </si>
-  <si>
-    <t>Seminar</t>
   </si>
   <si>
     <t>Remedial/Honours Course</t>
@@ -646,6 +643,12 @@
   </si>
   <si>
     <t>Open Elective -1 I with Python</t>
+  </si>
+  <si>
+    <t>Seminar - Review</t>
+  </si>
+  <si>
+    <t>Option 1: Major Project -Guide</t>
   </si>
 </sst>
 </file>
@@ -1056,28 +1059,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1088,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2">
         <v>70</v>
@@ -1114,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3">
         <v>70</v>
@@ -1140,7 +1143,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4">
         <v>70</v>
@@ -1166,7 +1169,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>70</v>
@@ -1192,7 +1195,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6">
         <v>70</v>
@@ -1218,7 +1221,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7">
         <v>70</v>
@@ -1244,7 +1247,7 @@
         <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8">
         <v>70</v>
@@ -1289,28 +1292,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1321,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2">
         <v>70</v>
@@ -1347,7 +1350,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3">
         <v>70</v>
@@ -1373,7 +1376,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4">
         <v>70</v>
@@ -1399,7 +1402,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>70</v>
@@ -1425,7 +1428,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6">
         <v>70</v>
@@ -1451,7 +1454,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7">
         <v>70</v>
@@ -1477,7 +1480,7 @@
         <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8">
         <v>70</v>
@@ -1521,28 +1524,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1553,7 +1556,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -1579,7 +1582,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -1605,7 +1608,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -1631,7 +1634,7 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -1657,7 +1660,7 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -1683,7 +1686,7 @@
         <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -1709,7 +1712,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -1735,7 +1738,7 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -1761,7 +1764,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10">
         <v>50</v>
@@ -1804,28 +1807,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1836,7 +1839,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -1862,7 +1865,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -1888,7 +1891,7 @@
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -1914,7 +1917,7 @@
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -1940,7 +1943,7 @@
         <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D6" s="1">
         <v>50</v>
@@ -1966,7 +1969,7 @@
         <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D7" s="1">
         <v>50</v>
@@ -2070,7 +2073,7 @@
         <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2096,7 +2099,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D12">
         <v>50</v>
@@ -2122,7 +2125,7 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D13">
         <v>50</v>
@@ -2148,7 +2151,7 @@
         <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="2">
         <v>50</v>
@@ -2191,28 +2194,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2223,7 +2226,7 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -2249,7 +2252,7 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3">
         <v>40</v>
@@ -2275,7 +2278,7 @@
         <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4">
         <v>40</v>
@@ -2301,7 +2304,7 @@
         <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>40</v>
@@ -2327,7 +2330,7 @@
         <v>80</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D6" s="1">
         <v>40</v>
@@ -2350,10 +2353,10 @@
         <v>76</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D7" s="1">
         <v>40</v>
@@ -2457,7 +2460,7 @@
         <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D11">
         <v>40</v>
@@ -2483,7 +2486,7 @@
         <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D12">
         <v>40</v>
@@ -2509,7 +2512,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D13" s="2">
         <v>40</v>
@@ -2551,28 +2554,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2583,7 +2586,7 @@
         <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -2609,7 +2612,7 @@
         <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3">
         <v>40</v>
@@ -2635,7 +2638,7 @@
         <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4">
         <v>40</v>
@@ -2661,7 +2664,7 @@
         <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>40</v>
@@ -2687,7 +2690,7 @@
         <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6">
         <v>40</v>
@@ -2713,7 +2716,7 @@
         <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7">
         <v>40</v>
@@ -2739,7 +2742,7 @@
         <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D8" s="2">
         <v>40</v>
@@ -2765,7 +2768,7 @@
         <v>106</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D9" s="3">
         <v>40</v>
@@ -2791,7 +2794,7 @@
         <v>105</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10" s="3">
         <v>40</v>
@@ -2895,7 +2898,7 @@
         <v>110</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="2">
         <v>40</v>
@@ -2921,7 +2924,7 @@
         <v>111</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="2">
         <v>40</v>
@@ -2944,7 +2947,7 @@
         <v>109</v>
       </c>
       <c r="B16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2975,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1D549B-B3E8-407F-8594-6DBABB4D89B9}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2993,28 +2996,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3022,10 +3025,10 @@
         <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" t="s">
-        <v>189</v>
+        <v>193</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -3045,13 +3048,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" t="s">
-        <v>189</v>
+        <v>194</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
       <c r="D3">
         <v>60</v>
@@ -3071,10 +3074,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3097,13 +3100,13 @@
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D5" s="2">
         <v>60</v>
@@ -3123,13 +3126,13 @@
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D6" s="1">
         <v>60</v>
@@ -3149,10 +3152,10 @@
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -3175,10 +3178,10 @@
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -3201,10 +3204,10 @@
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="4">
         <v>0</v>
@@ -3227,10 +3230,10 @@
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="C10" s="4">
         <v>0</v>
@@ -3253,10 +3256,10 @@
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="4">
         <v>0</v>
@@ -3279,10 +3282,10 @@
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="4">
         <v>0</v>
@@ -3305,10 +3308,10 @@
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" s="4">
         <v>0</v>
@@ -3331,13 +3334,13 @@
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="1">
         <v>60</v>
@@ -3357,10 +3360,10 @@
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -3383,13 +3386,13 @@
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D16" s="2">
         <v>60</v>
@@ -3409,10 +3412,10 @@
     </row>
     <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
@@ -3435,10 +3438,10 @@
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C18" s="4">
         <v>0</v>
@@ -3461,10 +3464,10 @@
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -3487,10 +3490,10 @@
     </row>
     <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C20" s="4">
         <v>0</v>
@@ -3513,10 +3516,10 @@
     </row>
     <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" s="4">
         <v>0</v>
@@ -3539,10 +3542,10 @@
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C22" s="4">
         <v>0</v>
@@ -3565,13 +3568,13 @@
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D23" s="4">
         <v>60</v>
@@ -3598,7 +3601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5407EBD7-2E39-401C-A46B-5C53E0C7EE30}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -3615,39 +3618,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D2" s="1">
         <v>60</v>
@@ -3667,13 +3670,13 @@
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D3" s="1">
         <v>60</v>
@@ -3693,10 +3696,10 @@
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>
@@ -3719,10 +3722,10 @@
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
@@ -3745,10 +3748,10 @@
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
@@ -3771,13 +3774,13 @@
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D7" s="2">
         <v>60</v>
@@ -3797,10 +3800,10 @@
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
@@ -3823,10 +3826,10 @@
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="4">
         <v>0</v>
@@ -3849,13 +3852,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" t="s">
         <v>172</v>
       </c>
-      <c r="B10" t="s">
-        <v>173</v>
-      </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -3875,10 +3878,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -3901,13 +3904,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -3927,10 +3930,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -3953,10 +3956,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14">
         <v>0</v>

</xml_diff>